<commit_message>
Cast C08 and C09. Made C10 sheet
</commit_message>
<xml_diff>
--- a/Charge 18 - C08.xlsx
+++ b/Charge 18 - C08.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Elements Data" sheetId="4" r:id="rId1"/>
@@ -4880,7 +4880,7 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -4920,7 +4920,7 @@
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="173" t="str">
         <f>"Actual  " &amp; 'Charge 18'!I3</f>
-        <v>Actual  Mg0Ca100</v>
+        <v>Actual  Mg65Zn30Ca5</v>
       </c>
       <c r="B3" s="174"/>
       <c r="C3" s="174"/>
@@ -4982,17 +4982,17 @@
       <c r="A6" s="26">
         <v>1</v>
       </c>
-      <c r="B6" s="105" t="str">
+      <c r="B6" s="105">
         <f>IF('Charge 18'!B14=0, "-", 'Charge 18'!B14)</f>
-        <v>-</v>
-      </c>
-      <c r="C6" s="137" t="str">
+        <v>3.8980000000000001</v>
+      </c>
+      <c r="C6" s="137">
         <f>IF('Charge 18'!E14=0,"-",'Charge 18'!E14)</f>
-        <v>-</v>
+        <v>23.437999999999999</v>
       </c>
       <c r="D6" s="137">
         <f>IF('Charge 18'!H14=0, "-", 'Charge 18'!H14)</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E6" s="137" t="str">
         <f>IF('Charge 18'!K14=0, "-", 'Charge 18'!K14)</f>
@@ -5004,7 +5004,7 @@
       </c>
       <c r="G6" s="138">
         <f>COUNTIF(B6:B20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H6" s="131" t="str">
         <f>B4</f>
@@ -5015,13 +5015,13 @@
       <c r="A7" s="27">
         <v>2</v>
       </c>
-      <c r="B7" s="108" t="str">
+      <c r="B7" s="108">
         <f>IF('Charge 18'!B15=0, "-", 'Charge 18'!B15)</f>
-        <v>-</v>
-      </c>
-      <c r="C7" s="107" t="str">
+        <v>5.3150000000000004</v>
+      </c>
+      <c r="C7" s="107">
         <f>IF('Charge 18'!E15=0,"-",'Charge 18'!E15)</f>
-        <v>-</v>
+        <v>22.641999999999999</v>
       </c>
       <c r="D7" s="107" t="str">
         <f>IF('Charge 18'!H15=0, "-", 'Charge 18'!H15)</f>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="G7" s="106">
         <f>COUNTIF(C6:C20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="151" t="str">
         <f>C4</f>
@@ -5048,13 +5048,13 @@
       <c r="A8" s="27">
         <v>3</v>
       </c>
-      <c r="B8" s="108" t="str">
+      <c r="B8" s="108">
         <f>IF('Charge 18'!B16=0, "-", 'Charge 18'!B16)</f>
-        <v>-</v>
-      </c>
-      <c r="C8" s="107" t="str">
+        <v>6.8150000000000004</v>
+      </c>
+      <c r="C8" s="107">
         <f>IF('Charge 18'!E16=0,"-",'Charge 18'!E16)</f>
-        <v>-</v>
+        <v>21.632999999999999</v>
       </c>
       <c r="D8" s="107" t="str">
         <f>IF('Charge 18'!H16=0, "-", 'Charge 18'!H16)</f>
@@ -5081,13 +5081,13 @@
       <c r="A9" s="27">
         <v>4</v>
       </c>
-      <c r="B9" s="108" t="str">
+      <c r="B9" s="108">
         <f>IF('Charge 18'!B17=0, "-", 'Charge 18'!B17)</f>
-        <v>-</v>
-      </c>
-      <c r="C9" s="107" t="str">
+        <v>7.149</v>
+      </c>
+      <c r="C9" s="107">
         <f>IF('Charge 18'!E17=0,"-",'Charge 18'!E17)</f>
-        <v>-</v>
+        <v>17.456</v>
       </c>
       <c r="D9" s="107" t="str">
         <f>IF('Charge 18'!H17=0, "-", 'Charge 18'!H17)</f>
@@ -5114,9 +5114,9 @@
       <c r="A10" s="27">
         <v>5</v>
       </c>
-      <c r="B10" s="108" t="str">
+      <c r="B10" s="108">
         <f>IF('Charge 18'!B18=0, "-", 'Charge 18'!B18)</f>
-        <v>-</v>
+        <v>7.1660000000000004</v>
       </c>
       <c r="C10" s="107" t="str">
         <f>IF('Charge 18'!E18=0,"-",'Charge 18'!E18)</f>
@@ -5147,9 +5147,9 @@
       <c r="A11" s="27">
         <v>6</v>
       </c>
-      <c r="B11" s="108" t="str">
+      <c r="B11" s="108">
         <f>IF('Charge 18'!B19=0, "-", 'Charge 18'!B19)</f>
-        <v>-</v>
+        <v>7.2839999999999998</v>
       </c>
       <c r="C11" s="107" t="str">
         <f>IF('Charge 18'!E19=0,"-",'Charge 18'!E19)</f>
@@ -5169,7 +5169,7 @@
       </c>
       <c r="G11" s="160">
         <f>COUNTIF(B6:F20, "&lt;&gt;-")</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H11" s="153" t="str">
         <f>G4</f>
@@ -5180,9 +5180,9 @@
       <c r="A12" s="27">
         <v>7</v>
       </c>
-      <c r="B12" s="108" t="str">
+      <c r="B12" s="108">
         <f>IF('Charge 18'!B20=0, "-", 'Charge 18'!B20)</f>
-        <v>-</v>
+        <v>7.4160000000000004</v>
       </c>
       <c r="C12" s="107" t="str">
         <f>IF('Charge 18'!E20=0,"-",'Charge 18'!E20)</f>
@@ -5206,9 +5206,9 @@
       <c r="A13" s="27">
         <v>8</v>
       </c>
-      <c r="B13" s="108" t="str">
+      <c r="B13" s="108">
         <f>IF('Charge 18'!B21=0, "-", 'Charge 18'!B21)</f>
-        <v>-</v>
+        <v>10.991</v>
       </c>
       <c r="C13" s="107" t="str">
         <f>IF('Charge 18'!E21=0,"-",'Charge 18'!E21)</f>
@@ -5232,9 +5232,9 @@
       <c r="A14" s="27">
         <v>9</v>
       </c>
-      <c r="B14" s="108" t="str">
+      <c r="B14" s="108">
         <f>IF('Charge 18'!B22=0, "-", 'Charge 18'!B22)</f>
-        <v>-</v>
+        <v>12.552</v>
       </c>
       <c r="C14" s="107" t="str">
         <f>IF('Charge 18'!E22=0,"-",'Charge 18'!E22)</f>
@@ -5416,15 +5416,15 @@
       </c>
       <c r="B21" s="77">
         <f>SUM(B6:B20)</f>
-        <v>0</v>
+        <v>68.586000000000013</v>
       </c>
       <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
-        <v>0</v>
+        <v>85.168999999999997</v>
       </c>
       <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E21" s="69">
         <f>SUM(E6:E20)</f>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="G21" s="144">
         <f>SUM(B21:F21)</f>
-        <v>3.5110000000000001</v>
+        <v>162.45499999999998</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5445,15 +5445,15 @@
       </c>
       <c r="B22" s="145">
         <f>'Charge 18'!F4</f>
-        <v>27.677</v>
+        <v>68.59</v>
       </c>
       <c r="C22" s="135">
         <f>'Charge 18'!F5</f>
-        <v>34.363</v>
+        <v>85.16</v>
       </c>
       <c r="D22" s="135">
         <f>'Charge 18'!F6</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E22" s="135">
         <f>'Charge 18'!F7</f>
@@ -5465,7 +5465,7 @@
       </c>
       <c r="G22" s="70">
         <f>SUM(B22:F22)</f>
-        <v>65.551000000000002</v>
+        <v>162.44999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5474,11 +5474,11 @@
       </c>
       <c r="B23" s="146">
         <f>B21-B22</f>
-        <v>-27.677</v>
+        <v>-3.9999999999906777E-3</v>
       </c>
       <c r="C23" s="140">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>-34.363</v>
+        <v>9.0000000000003411E-3</v>
       </c>
       <c r="D23" s="140">
         <f t="shared" si="0"/>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-62.04</v>
+        <v>4.9999999999954525E-3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5518,9 +5518,9 @@
   </sheetPr>
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg0Ca100</v>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5683,11 +5683,11 @@
       </c>
       <c r="F4" s="69">
         <f>IF($F$9=0, ROUND($F$10*E4, 3), ROUND(E4*$F$9, 3))</f>
-        <v>27.677</v>
+        <v>68.59</v>
       </c>
       <c r="G4" s="70">
         <f>IFERROR(F4/U4, 0)</f>
-        <v>15.924626006904488</v>
+        <v>39.464902186421178</v>
       </c>
       <c r="I4" s="71" t="str">
         <f>$Q$4</f>
@@ -5696,19 +5696,19 @@
       <c r="J4" s="26"/>
       <c r="K4" s="72">
         <f>B29</f>
-        <v>0</v>
+        <v>68.586000000000013</v>
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0</v>
+        <v>0.42218460496752958</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>0</v>
+        <v>1.7370277925016647E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0</v>
+        <v>0.64996480387783218</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5780,11 +5780,11 @@
       </c>
       <c r="F5" s="69">
         <f t="shared" ref="F5:F8" si="0">IF($F$9=0, ROUND($F$10*E5, 3), ROUND(E5*$F$9, 3))</f>
-        <v>34.363</v>
+        <v>85.16</v>
       </c>
       <c r="G5" s="70">
         <f>IFERROR(F5/U5, 0)</f>
-        <v>4.8127450980392155</v>
+        <v>11.927170868347339</v>
       </c>
       <c r="I5" s="71" t="str">
         <f>$Q$5</f>
@@ -5793,19 +5793,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>0</v>
+        <v>85.168999999999997</v>
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0</v>
+        <v>0.52426210335169743</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>0</v>
+        <v>8.0184470244363485E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0</v>
+        <v>0.30003597928255737</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5877,11 +5877,11 @@
       </c>
       <c r="F6" s="69">
         <f t="shared" si="0"/>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="G6" s="70">
         <f>IFERROR(F6/U6, 0)</f>
-        <v>2.2651612903225806</v>
+        <v>5.6129032258064511</v>
       </c>
       <c r="I6" s="71" t="str">
         <f>$Q$6</f>
@@ -5890,19 +5890,19 @@
       <c r="J6" s="27"/>
       <c r="K6" s="77">
         <f>H29</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>1</v>
+        <v>5.3553291680773135E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>1.3362266500517273E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>1</v>
+        <v>4.9999216839610318E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="G9" s="144">
         <f>SUM(G4:G8)</f>
-        <v>23.002532395266286</v>
+        <v>57.004976280574965</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="79" t="s">
@@ -6178,7 +6178,7 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>3.5110000000000001</v>
+        <v>162.45499999999998</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
@@ -6186,11 +6186,11 @@
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>2.6724951599504724E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>111</v>
@@ -6232,10 +6232,10 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F10" s="158">
         <f>G10*U9</f>
-        <v>65.55</v>
+        <v>162.45000000000002</v>
       </c>
       <c r="G10" s="9">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="B14" s="106">
         <f>A!C2</f>
-        <v>0</v>
+        <v>3.8980000000000001</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="126">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>0</v>
+        <v>23.437999999999999</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="126">
@@ -6357,7 +6357,7 @@
       </c>
       <c r="H14" s="106">
         <f>'C'!C2</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="I14" s="107"/>
       <c r="J14" s="126">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="B15" s="106">
         <f>A!C3</f>
-        <v>0</v>
+        <v>5.3150000000000004</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="126">
@@ -6402,7 +6402,7 @@
       </c>
       <c r="E15" s="106">
         <f>B!C3</f>
-        <v>0</v>
+        <v>22.641999999999999</v>
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="126">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B16" s="106">
         <f>A!C4</f>
-        <v>0</v>
+        <v>6.8150000000000004</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="126">
@@ -6455,7 +6455,7 @@
       </c>
       <c r="E16" s="106">
         <f>B!C4</f>
-        <v>0</v>
+        <v>21.632999999999999</v>
       </c>
       <c r="F16" s="107"/>
       <c r="G16" s="126">
@@ -6500,7 +6500,7 @@
       </c>
       <c r="B17" s="106">
         <f>A!C5</f>
-        <v>0</v>
+        <v>7.149</v>
       </c>
       <c r="C17" s="107"/>
       <c r="D17" s="126">
@@ -6508,7 +6508,7 @@
       </c>
       <c r="E17" s="106">
         <f>B!C5</f>
-        <v>0</v>
+        <v>17.456</v>
       </c>
       <c r="F17" s="107"/>
       <c r="G17" s="126">
@@ -6553,7 +6553,7 @@
       </c>
       <c r="B18" s="106">
         <f>A!C6</f>
-        <v>0</v>
+        <v>7.1660000000000004</v>
       </c>
       <c r="C18" s="107"/>
       <c r="D18" s="126">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="B19" s="106">
         <f>A!C7</f>
-        <v>0</v>
+        <v>7.2839999999999998</v>
       </c>
       <c r="C19" s="107"/>
       <c r="D19" s="126">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="B20" s="106">
         <f>A!C8</f>
-        <v>0</v>
+        <v>7.4160000000000004</v>
       </c>
       <c r="C20" s="107"/>
       <c r="D20" s="126">
@@ -6714,7 +6714,7 @@
       </c>
       <c r="B21" s="106">
         <f>A!C9</f>
-        <v>0</v>
+        <v>10.991</v>
       </c>
       <c r="C21" s="107"/>
       <c r="D21" s="126">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="B22" s="106">
         <f>A!C10</f>
-        <v>0</v>
+        <v>12.552</v>
       </c>
       <c r="C22" s="107"/>
       <c r="D22" s="126">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="B29" s="110">
         <f>SUM(B14:B28)</f>
-        <v>0</v>
+        <v>68.586000000000013</v>
       </c>
       <c r="C29" s="107"/>
       <c r="D29" s="109" t="s">
@@ -7067,7 +7067,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>0</v>
+        <v>85.168999999999997</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="H29" s="110">
         <f>SUM(H14:H28)</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="I29" s="107"/>
       <c r="J29" s="109" t="s">
@@ -7100,7 +7100,7 @@
       </c>
       <c r="B30" s="113">
         <f>B29-$F$4</f>
-        <v>-27.677</v>
+        <v>-3.9999999999906777E-3</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="112" t="s">
@@ -7108,7 +7108,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>-34.363</v>
+        <v>9.0000000000003411E-3</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -8522,7 +8522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8557,37 +8557,37 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="166">
-        <v>3.9849999999999999</v>
+        <v>3.8980000000000001</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <v>3.8980000000000001</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>68.586000000000013</v>
       </c>
       <c r="E2" s="127" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="129">
         <f>'Charge 18'!F4</f>
-        <v>27.677</v>
+        <v>68.59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="166">
-        <v>5.4009999999999998</v>
+        <v>5.3150000000000004</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <v>5.3150000000000004</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="127" t="s">
@@ -8595,19 +8595,19 @@
       </c>
       <c r="F3" s="129">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>68.586000000000013</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="166">
-        <v>5.5540000000000003</v>
+        <v>6.8150000000000004</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f>IF(A4=0, 0, A4*B4)</f>
-        <v>0</v>
+        <v>6.8150000000000004</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="127" t="s">
@@ -8615,86 +8615,86 @@
       </c>
       <c r="F4" s="129">
         <f>F3-F2</f>
-        <v>-27.677</v>
+        <v>-3.9999999999906777E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>5.6260000000000003</v>
+        <v>7.149</v>
       </c>
       <c r="B5" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>IF(A5=0, 0, A5*B5)</f>
-        <v>0</v>
+        <v>7.149</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>5.64</v>
+        <v>7.1660000000000004</v>
       </c>
       <c r="B6" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f>IF(A6=0, 0, A6*B6)</f>
-        <v>0</v>
+        <v>7.1660000000000004</v>
       </c>
       <c r="E6" s="167"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>5.7</v>
+        <v>7.2839999999999998</v>
       </c>
       <c r="B7" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f>IF(A7=0, 0, A7*B7)</f>
-        <v>0</v>
+        <v>7.2839999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="166">
-        <v>5.9320000000000004</v>
+        <v>7.4160000000000004</v>
       </c>
       <c r="B8" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f>IF(A8=0, 0, A8*B8)</f>
-        <v>0</v>
+        <v>7.4160000000000004</v>
       </c>
       <c r="E8" s="167"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="166">
-        <v>6.2210000000000001</v>
+        <v>10.991</v>
       </c>
       <c r="B9" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f>IF(A9=0, 0, A9*B9)</f>
-        <v>0</v>
+        <v>10.991</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="166">
-        <v>6.4550000000000001</v>
+        <v>12.552</v>
       </c>
       <c r="B10" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <f>IF(A10=0, 0, A10*B10)</f>
-        <v>0</v>
+        <v>12.552</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="166">
-        <v>6.5289999999999999</v>
+        <v>5.4939999999999998</v>
       </c>
       <c r="B11" s="125">
         <v>0</v>
@@ -8706,7 +8706,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="166">
-        <v>6.7119999999999997</v>
+        <v>5.5179999999999998</v>
       </c>
       <c r="B12" s="125">
         <v>0</v>
@@ -8718,7 +8718,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="166">
-        <v>6.8869999999999996</v>
+        <v>5.5449999999999999</v>
       </c>
       <c r="B13" s="125">
         <v>0</v>
@@ -8730,7 +8730,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="166">
-        <v>7.1079999999999997</v>
+        <v>5.5990000000000002</v>
       </c>
       <c r="B14" s="125">
         <v>0</v>
@@ -8742,7 +8742,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="166">
-        <v>7.2359999999999998</v>
+        <v>5.8650000000000002</v>
       </c>
       <c r="B15" s="125">
         <v>0</v>
@@ -8754,7 +8754,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="166">
-        <v>7.26</v>
+        <v>6.1580000000000004</v>
       </c>
       <c r="B16" s="125">
         <v>0</v>
@@ -8766,7 +8766,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="166">
-        <v>7.3710000000000004</v>
+        <v>6.3570000000000002</v>
       </c>
       <c r="B17" s="125">
         <v>0</v>
@@ -8778,7 +8778,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="166">
-        <v>7.4859999999999998</v>
+        <v>6.4690000000000003</v>
       </c>
       <c r="B18" s="125">
         <v>0</v>
@@ -8790,7 +8790,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="166">
-        <v>7.7169999999999996</v>
+        <v>6.6529999999999996</v>
       </c>
       <c r="B19" s="125">
         <v>0</v>
@@ -8802,7 +8802,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="166">
-        <v>7.75</v>
+        <v>7.0270000000000001</v>
       </c>
       <c r="B20" s="125">
         <v>0</v>
@@ -8814,7 +8814,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="166">
-        <v>8.8819999999999997</v>
+        <v>7.6379999999999999</v>
       </c>
       <c r="B21" s="125">
         <v>0</v>
@@ -8826,7 +8826,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="166">
-        <v>11.09</v>
+        <v>7.6779999999999999</v>
       </c>
       <c r="B22" s="125">
         <v>0</v>
@@ -8838,7 +8838,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="166">
-        <v>11.398</v>
+        <v>8.7910000000000004</v>
       </c>
       <c r="B23" s="125">
         <v>0</v>
@@ -8850,7 +8850,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="166">
-        <v>12.666</v>
+        <v>11.292</v>
       </c>
       <c r="B24" s="125">
         <v>0</v>
@@ -9133,7 +9133,7 @@
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9150,7 +9150,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9185,80 +9185,80 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>11.923999999999999</v>
+        <v>23.437999999999999</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <v>23.437999999999999</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>85.168999999999997</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 18'!F5</f>
-        <v>34.363</v>
+        <v>85.16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>12.84</v>
+        <v>22.641999999999999</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <v>22.641999999999999</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>85.168999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>16.696999999999999</v>
+        <v>21.632999999999999</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f>IF(A4=0, 0, A4*B4)</f>
-        <v>0</v>
+        <v>21.632999999999999</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-34.363</v>
+        <v>9.0000000000003411E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>17.350999999999999</v>
+        <v>17.456</v>
       </c>
       <c r="B5" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>IF(A5=0, 0, A5*B5)</f>
-        <v>0</v>
+        <v>17.456</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>17.641999999999999</v>
+        <v>11.855</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
@@ -9270,7 +9270,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="125">
-        <v>18.521999999999998</v>
+        <v>12.72</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
@@ -9282,7 +9282,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="125">
-        <v>19.594999999999999</v>
+        <v>16.52</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
@@ -9294,7 +9294,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="125">
-        <v>20.327999999999999</v>
+        <v>17.268000000000001</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
@@ -9306,7 +9306,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="125">
-        <v>20.736999999999998</v>
+        <v>18.271999999999998</v>
       </c>
       <c r="B10" s="125">
         <v>0</v>
@@ -9318,7 +9318,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="125">
-        <v>21.207000000000001</v>
+        <v>19.414000000000001</v>
       </c>
       <c r="B11" s="125">
         <v>0</v>
@@ -9330,7 +9330,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="125">
-        <v>21.754999999999999</v>
+        <v>20.16</v>
       </c>
       <c r="B12" s="125">
         <v>0</v>
@@ -9342,7 +9342,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="125">
-        <v>22.9</v>
+        <v>20.597000000000001</v>
       </c>
       <c r="B13" s="125">
         <v>0</v>
@@ -9354,7 +9354,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="125">
-        <v>23.218</v>
+        <v>21.074999999999999</v>
       </c>
       <c r="B14" s="125">
         <v>0</v>
@@ -9366,7 +9366,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="125">
-        <v>23.518000000000001</v>
+        <v>23.068999999999999</v>
       </c>
       <c r="B15" s="125">
         <v>0</v>
@@ -9378,7 +9378,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="125">
-        <v>24.568999999999999</v>
+        <v>24.469000000000001</v>
       </c>
       <c r="B16" s="125">
         <v>0</v>
@@ -9741,7 +9741,7 @@
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="C1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9758,7 +9758,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9793,25 +9793,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 18'!F6</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9828,7 +9828,7 @@
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>3.5110000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>